<commit_message>
highlighted new/old biospecimen querries
</commit_message>
<xml_diff>
--- a/managed_queries.xlsx
+++ b/managed_queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petersjm/Documents/dataFlattening/flatteningRequests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E263852-02A5-784A-B050-6F54D041C2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778EF87C-A73B-E143-BD5E-B2D0DB0AC4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1160" windowWidth="30240" windowHeight="11840" xr2:uid="{F9774F69-D19B-9642-B7EB-8880EC4E13B4}"/>
   </bookViews>
@@ -656,7 +656,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A3" activeCellId="1" sqref="A2:XFD2 A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added M1V1 & M1V2 queries to managed_queries.xlsx
</commit_message>
<xml_diff>
--- a/managed_queries.xlsx
+++ b/managed_queries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petersjm/Documents/dataFlattening/flatteningRequests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778EF87C-A73B-E143-BD5E-B2D0DB0AC4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75744BE6-D9E1-8448-B80C-61A63CC076DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1160" windowWidth="30240" windowHeight="11840" xr2:uid="{F9774F69-D19B-9642-B7EB-8880EC4E13B4}"/>
+    <workbookView xWindow="-35200" yWindow="1020" windowWidth="30240" windowHeight="11840" xr2:uid="{F9774F69-D19B-9642-B7EB-8880EC4E13B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="66">
   <si>
     <t>flatM2_JP_SA</t>
   </si>
@@ -213,6 +213,27 @@
   </si>
   <si>
     <t>https://github.com/Analyticsphere/flatteningRequests/tree/main/queryGenerators/recruitment</t>
+  </si>
+  <si>
+    <t>flatM1V2_JP_SA</t>
+  </si>
+  <si>
+    <t>M1.flatM1V2_JP_SA</t>
+  </si>
+  <si>
+    <t>https://github.com/Analyticsphere/flatteningRequests/tree/main/queryGenerators/M1V1</t>
+  </si>
+  <si>
+    <t>https://github.com/Analyticsphere/flatteningRequests/tree/main/queryGenerators/M1V2</t>
+  </si>
+  <si>
+    <t>flatM1V1_JP_SA</t>
+  </si>
+  <si>
+    <t>scheduled</t>
+  </si>
+  <si>
+    <t>M1.flatM1V1_JP_SA</t>
   </si>
 </sst>
 </file>
@@ -306,7 +327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -338,6 +359,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -653,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D16EF72-59FA-4949-AD1C-60CEF9E055C7}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" activeCellId="1" sqref="A2:XFD2 A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L39" sqref="I36:L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -664,19 +686,20 @@
     <col min="1" max="1" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="60.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="83.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="55.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="83.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="55.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
@@ -687,34 +710,37 @@
         <v>53</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="10" customFormat="1" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="10" customFormat="1" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
@@ -724,23 +750,26 @@
       <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="11" t="s">
+      <c r="D2" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>36</v>
       </c>
@@ -750,23 +779,26 @@
       <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L3" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>36</v>
       </c>
@@ -776,32 +808,35 @@
       <c r="C4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="18" t="s">
+      <c r="D4" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>34</v>
-      </c>
       <c r="H4" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="J4" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="K4" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="L4" s="20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -811,754 +846,1074 @@
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="L5" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>34</v>
+      <c r="D6" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>34</v>
+      <c r="D7" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>34</v>
+      <c r="G8" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="L10" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="D11" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="6" t="s">
+      <c r="G11" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="K11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="L11" s="14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="10" t="s">
+      <c r="D12" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="I12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="10"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D13" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="I13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
+      <c r="J13" s="10"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="M13" s="10"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B14" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="18" t="s">
+      <c r="D14" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="16" t="s">
+      <c r="H14" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="J14" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="K14" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="K12" s="20" t="s">
+      <c r="L14" s="20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="M14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>34</v>
+      <c r="D15" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L15" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>34</v>
+      <c r="D16" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="D17" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="G21" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K17" s="9" t="s">
+      <c r="L21" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="11" t="s">
+      <c r="D22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="H22" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="I22" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K18" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="M22" s="10"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B23" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D23" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="F23" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="G23" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="H23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="I23" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K19" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="M23" s="10"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B24" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="18" t="s">
+      <c r="D24" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="16" t="s">
+      <c r="H24" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="J24" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="K24" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="20" t="s">
+      <c r="L24" s="20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="M24" s="16"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K24" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>34</v>
+      <c r="D25" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L25" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="D26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L31" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H26" s="1" t="s">
+      <c r="G32" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="K32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K26" s="9" t="s">
+      <c r="L32" s="9" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L27">
-    <sortCondition ref="C1:C27"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M33">
+    <sortCondition ref="C1:C33"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K4" r:id="rId1" xr:uid="{058491E3-C290-9048-B091-B59ECBB73784}"/>
-    <hyperlink ref="K20" r:id="rId2" xr:uid="{E9D970B4-BAB6-B649-8DE5-D99F38F00DC0}"/>
-    <hyperlink ref="K5" r:id="rId3" xr:uid="{85D7F2CC-2E6B-D84D-877C-002A68269A86}"/>
-    <hyperlink ref="K12" r:id="rId4" xr:uid="{76E52B4E-7CA3-6D49-8B11-9C8CE6281F00}"/>
-    <hyperlink ref="K12:K13" r:id="rId5" display="https://github.com/Analyticsphere/flatteningRequests/tree/main/queryGenerators/M1" xr:uid="{D9CE1DBA-118F-4943-8076-068343794CE8}"/>
-    <hyperlink ref="K13" r:id="rId6" xr:uid="{8D812808-DAC4-3847-9DB1-842BD1E085D6}"/>
-    <hyperlink ref="K21" r:id="rId7" xr:uid="{D06B47F9-22E3-4B48-B7A1-B20C2E670A0D}"/>
-    <hyperlink ref="K6" r:id="rId8" xr:uid="{817A1287-356B-A442-9E9E-BF69A45B1833}"/>
-    <hyperlink ref="K14" r:id="rId9" xr:uid="{77E1CAC0-27C1-8043-94E5-D6C5E3ED8133}"/>
-    <hyperlink ref="K22" r:id="rId10" xr:uid="{75D8D0B5-4E28-CE46-9748-741B72F074F8}"/>
-    <hyperlink ref="K23" r:id="rId11" xr:uid="{16BD0BC9-350D-A143-B902-10E386036971}"/>
-    <hyperlink ref="K7" r:id="rId12" xr:uid="{3C611B71-4868-F74A-8132-84350C2A5A0D}"/>
-    <hyperlink ref="K15" r:id="rId13" xr:uid="{9E2E2056-D9B4-0C40-BA13-A1DA4A6A0439}"/>
-    <hyperlink ref="K24" r:id="rId14" xr:uid="{07272495-6373-5142-A2DA-63AA50B558E1}"/>
-    <hyperlink ref="K8" r:id="rId15" xr:uid="{CB145F19-CEB0-1542-9685-E9A737B8045F}"/>
-    <hyperlink ref="K16" r:id="rId16" xr:uid="{907D22EF-A053-EE4F-85BE-718A86A6ED06}"/>
-    <hyperlink ref="K25" r:id="rId17" xr:uid="{BB6FB076-B428-394C-A3C9-17ECEDA34514}"/>
-    <hyperlink ref="K9" r:id="rId18" xr:uid="{33666846-E51B-804B-B6E1-A342BF60CEC0}"/>
-    <hyperlink ref="K17" r:id="rId19" xr:uid="{0404A9E9-E1FD-B445-904C-25936CF5E9F2}"/>
-    <hyperlink ref="K26" r:id="rId20" xr:uid="{0C4D4899-557E-1B4B-90D3-2CC853468758}"/>
+    <hyperlink ref="L4" r:id="rId1" xr:uid="{058491E3-C290-9048-B091-B59ECBB73784}"/>
+    <hyperlink ref="L24" r:id="rId2" xr:uid="{E9D970B4-BAB6-B649-8DE5-D99F38F00DC0}"/>
+    <hyperlink ref="L5" r:id="rId3" xr:uid="{85D7F2CC-2E6B-D84D-877C-002A68269A86}"/>
+    <hyperlink ref="L14" r:id="rId4" xr:uid="{76E52B4E-7CA3-6D49-8B11-9C8CE6281F00}"/>
+    <hyperlink ref="L12:L13" r:id="rId5" display="https://github.com/Analyticsphere/flatteningRequests/tree/main/queryGenerators/M1" xr:uid="{D9CE1DBA-118F-4943-8076-068343794CE8}"/>
+    <hyperlink ref="L15" r:id="rId6" xr:uid="{8D812808-DAC4-3847-9DB1-842BD1E085D6}"/>
+    <hyperlink ref="L25" r:id="rId7" xr:uid="{D06B47F9-22E3-4B48-B7A1-B20C2E670A0D}"/>
+    <hyperlink ref="L8" r:id="rId8" xr:uid="{817A1287-356B-A442-9E9E-BF69A45B1833}"/>
+    <hyperlink ref="L18" r:id="rId9" xr:uid="{77E1CAC0-27C1-8043-94E5-D6C5E3ED8133}"/>
+    <hyperlink ref="L28" r:id="rId10" xr:uid="{75D8D0B5-4E28-CE46-9748-741B72F074F8}"/>
+    <hyperlink ref="L29" r:id="rId11" xr:uid="{16BD0BC9-350D-A143-B902-10E386036971}"/>
+    <hyperlink ref="L9" r:id="rId12" xr:uid="{3C611B71-4868-F74A-8132-84350C2A5A0D}"/>
+    <hyperlink ref="L19" r:id="rId13" xr:uid="{9E2E2056-D9B4-0C40-BA13-A1DA4A6A0439}"/>
+    <hyperlink ref="L30" r:id="rId14" xr:uid="{07272495-6373-5142-A2DA-63AA50B558E1}"/>
+    <hyperlink ref="L10" r:id="rId15" xr:uid="{CB145F19-CEB0-1542-9685-E9A737B8045F}"/>
+    <hyperlink ref="L20" r:id="rId16" xr:uid="{907D22EF-A053-EE4F-85BE-718A86A6ED06}"/>
+    <hyperlink ref="L31" r:id="rId17" xr:uid="{BB6FB076-B428-394C-A3C9-17ECEDA34514}"/>
+    <hyperlink ref="L11" r:id="rId18" xr:uid="{33666846-E51B-804B-B6E1-A342BF60CEC0}"/>
+    <hyperlink ref="L21" r:id="rId19" xr:uid="{0404A9E9-E1FD-B445-904C-25936CF5E9F2}"/>
+    <hyperlink ref="L32" r:id="rId20" xr:uid="{0C4D4899-557E-1B4B-90D3-2CC853468758}"/>
+    <hyperlink ref="L16" r:id="rId21" xr:uid="{B15DDFE5-74FA-9440-83DE-7F191CA764C0}"/>
+    <hyperlink ref="L28:L29" r:id="rId22" display="https://github.com/Analyticsphere/flatteningRequests/tree/main/queryGenerators/M1V2" xr:uid="{658D29A2-6936-BD4B-99FA-015CA88A87C8}"/>
+    <hyperlink ref="L6" r:id="rId23" xr:uid="{69242CFD-0ACE-F642-812D-3901B86AA06B}"/>
+    <hyperlink ref="L26" r:id="rId24" xr:uid="{3A1665F7-D0D3-8141-8EBA-D9954114A915}"/>
+    <hyperlink ref="L17" r:id="rId25" xr:uid="{77901A03-982C-A148-A0DB-A34FBD7A65F4}"/>
+    <hyperlink ref="L7" r:id="rId26" xr:uid="{75310C88-48B7-984B-B490-2C75D9A9844C}"/>
+    <hyperlink ref="L27" r:id="rId27" xr:uid="{909EB73F-505C-CC46-B686-AF1E0AD0A9A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>